<commit_message>
Adding Linux numbers to results of 2016/04/06
</commit_message>
<xml_diff>
--- a/results/2016-04-06/Summary.xlsx
+++ b/results/2016-04-06/Summary.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\DavidObando\aspnet-memtest\results\2016-04-05\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\DavidObando\aspnet-memtest\results\2016-04-06\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23445" windowHeight="12225"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23445" windowHeight="12225" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Windows" sheetId="1" r:id="rId1"/>
+    <sheet name="Linux" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="35">
   <si>
     <t>Platform</t>
   </si>
@@ -106,6 +107,31 @@
   <si>
     <t>wrk -c 256 -t 32 -d 10 -s ./scripts/pipeline.lua http://10.194.216.73:5000/ -- 16</t>
   </si>
+  <si>
+    <t>Before Load</t>
+  </si>
+  <si>
+    <t>After Load</t>
+  </si>
+  <si>
+    <t>VSIZE</t>
+  </si>
+  <si>
+    <t>RSS</t>
+  </si>
+  <si>
+    <t>Ratio vs Best (VSIZE)</t>
+  </si>
+  <si>
+    <t>Ratio vs Best (RSS)</t>
+  </si>
+  <si>
+    <t>ps -o rss,vsize,command -u asplab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wrk -c 256 -t 32 -d 10 -s ./scripts/pipeline.lua http://10.194.217.77:5000/ -- 16
+</t>
+  </si>
 </sst>
 </file>
 
@@ -180,14 +206,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
@@ -198,23 +221,33 @@
     <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="13">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="13" formatCode="0%"/>
     </dxf>
     <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -237,13 +270,18 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2599,14 +2637,14 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="BeforeLoad" displayName="BeforeLoad" ref="A2:F12" totalsRowShown="0">
   <autoFilter ref="A2:F12"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Platform" dataDxfId="2"/>
+    <tableColumn id="1" name="Platform" dataDxfId="12"/>
     <tableColumn id="2" name="Committed"/>
     <tableColumn id="3" name="Private Bytes"/>
     <tableColumn id="4" name="Working Set"/>
-    <tableColumn id="5" name="Ratio vs Best (WS)" dataDxfId="7">
+    <tableColumn id="5" name="Ratio vs Best (WS)" dataDxfId="11">
       <calculatedColumnFormula>ROUND(BeforeLoad[[#This Row],[Working Set]]/MIN(BeforeLoad[Working Set]),1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Ratio vs Best (PB)" dataDxfId="6">
+    <tableColumn id="6" name="Ratio vs Best (PB)" dataDxfId="10">
       <calculatedColumnFormula>ROUND(BeforeLoad[[#This Row],[Private Bytes]]/MIN(BeforeLoad[Private Bytes]),1)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2621,19 +2659,19 @@
     <sortCondition ref="A24:A38"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="1" name="Platform" dataDxfId="1"/>
+    <tableColumn id="1" name="Platform" dataDxfId="9"/>
     <tableColumn id="8" name="RPS"/>
     <tableColumn id="5" name="Avg latency (ms)"/>
     <tableColumn id="2" name="Committed"/>
     <tableColumn id="3" name="Private Bytes"/>
     <tableColumn id="4" name="Working Set"/>
-    <tableColumn id="9" name="Ratio vs Best (WS)" dataDxfId="5">
+    <tableColumn id="9" name="Ratio vs Best (WS)" dataDxfId="8">
       <calculatedColumnFormula>ROUND(AfterLoad[[#This Row],[Working Set]]/MIN(AfterLoad[Working Set]),1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Ratio vs Best (PB)" dataDxfId="4">
+    <tableColumn id="6" name="Ratio vs Best (PB)" dataDxfId="7">
       <calculatedColumnFormula>ROUND(AfterLoad[[#This Row],[Private Bytes]]/MIN(AfterLoad[Private Bytes]),1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Ratio vs Best (RPS)" dataDxfId="3">
+    <tableColumn id="7" name="Ratio vs Best (RPS)" dataDxfId="6">
       <calculatedColumnFormula>ROUND(AfterLoad[[#This Row],[RPS]]/MAX(AfterLoad[RPS]),2)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2647,7 +2685,48 @@
   <tableColumns count="3">
     <tableColumn id="1" name="Platform"/>
     <tableColumn id="4" name="Command"/>
-    <tableColumn id="5" name="Server CPU utilization" dataDxfId="0"/>
+    <tableColumn id="5" name="Server CPU utilization" dataDxfId="5"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:E6" totalsRowShown="0">
+  <autoFilter ref="A2:E6"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Platform"/>
+    <tableColumn id="2" name="VSIZE"/>
+    <tableColumn id="3" name="RSS"/>
+    <tableColumn id="5" name="Ratio vs Best (VSIZE)" dataDxfId="4">
+      <calculatedColumnFormula>ROUND(Table1[[#This Row],[VSIZE]]/MIN(Table1[VSIZE]),1)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" name="Ratio vs Best (RSS)" dataDxfId="1">
+      <calculatedColumnFormula>ROUND(Table1[[#This Row],[RSS]]/MIN(Table1[RSS]),1)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A11:H15" totalsRowShown="0">
+  <autoFilter ref="A11:H15"/>
+  <tableColumns count="8">
+    <tableColumn id="1" name="Platform"/>
+    <tableColumn id="2" name="RPS"/>
+    <tableColumn id="3" name="Avg latency (ms)"/>
+    <tableColumn id="4" name="VSIZE"/>
+    <tableColumn id="5" name="RSS"/>
+    <tableColumn id="7" name="Ratio vs Best (VSIZE)" dataDxfId="0">
+      <calculatedColumnFormula>ROUND(Table4[[#This Row],[VSIZE]]/MIN(Table4[VSIZE]),1)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" name="Ratio vs Best (RSS)" dataDxfId="3">
+      <calculatedColumnFormula>ROUND(Table4[[#This Row],[RSS]]/MIN(Table4[RSS]),1)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" name="Ratio vs Best (RPS)" dataDxfId="2">
+      <calculatedColumnFormula>ROUND(Table4[[#This Row],[RPS]]/MAX(Table4[RPS]),1)</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2952,8 +3031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2979,9 +3058,9 @@
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -3004,7 +3083,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B3">
@@ -3026,7 +3105,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>24</v>
       </c>
       <c r="B4">
@@ -3048,7 +3127,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B5">
@@ -3070,7 +3149,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B6">
@@ -3092,7 +3171,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B7">
@@ -3114,7 +3193,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B8">
@@ -3136,7 +3215,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B9">
@@ -3158,7 +3237,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B10">
@@ -3180,7 +3259,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B11">
@@ -3202,7 +3281,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B12">
@@ -3258,7 +3337,7 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B18">
@@ -3290,7 +3369,7 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B19">
@@ -3322,7 +3401,7 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B20">
@@ -3354,7 +3433,7 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B21">
@@ -3386,7 +3465,7 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B22">
@@ -3418,7 +3497,7 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B23">
@@ -3450,7 +3529,7 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B24">
@@ -3482,7 +3561,7 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B25">
@@ -3514,7 +3593,7 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
+      <c r="A26" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B26">
@@ -3546,7 +3625,7 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B27">
@@ -3578,10 +3657,10 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="6"/>
+      <c r="A30" s="5"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="7" t="s">
+      <c r="A31" s="6" t="s">
         <v>18</v>
       </c>
     </row>
@@ -3597,24 +3676,24 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
+      <c r="A33" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B33" t="s">
         <v>26</v>
       </c>
-      <c r="C33" s="8">
+      <c r="C33" s="7">
         <v>0.85</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
+      <c r="A34" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B34" t="s">
         <v>25</v>
       </c>
-      <c r="C34" s="8">
+      <c r="C34" s="7">
         <v>0.98</v>
       </c>
     </row>
@@ -3625,91 +3704,88 @@
       <c r="B35" t="s">
         <v>26</v>
       </c>
-      <c r="C35" s="8">
+      <c r="C35" s="7">
         <v>0.95</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
+      <c r="A36" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B36" t="s">
         <v>26</v>
       </c>
-      <c r="C36" s="8">
+      <c r="C36" s="7">
         <v>0.8</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
+      <c r="A37" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B37" t="s">
         <v>26</v>
       </c>
-      <c r="C37" s="8">
+      <c r="C37" s="7">
         <v>0.95</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="5" t="s">
+      <c r="A38" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B38" t="s">
         <v>26</v>
       </c>
-      <c r="C38" s="8">
+      <c r="C38" s="7">
         <v>0.85</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="5" t="s">
+      <c r="A39" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B39" t="s">
         <v>26</v>
       </c>
-      <c r="C39" s="8">
+      <c r="C39" s="7">
         <v>0.95</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="5" t="s">
+      <c r="A40" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B40" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="8">
+      <c r="C40" s="7">
         <v>0.85</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="5" t="s">
+      <c r="A41" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B41" t="s">
         <v>26</v>
       </c>
-      <c r="C41" s="8">
+      <c r="C41" s="7">
         <v>0.95</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="5" t="s">
+      <c r="A42" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B42" t="s">
         <v>26</v>
       </c>
-      <c r="C42" s="8">
+      <c r="C42" s="7">
         <v>0.8</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="E1:G1"/>
-  </mergeCells>
   <conditionalFormatting sqref="E3:F12">
     <cfRule type="dataBar" priority="10">
       <dataBar>
@@ -3833,4 +3909,434 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="46.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" customWidth="1"/>
+    <col min="9" max="9" width="19.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>22216956</v>
+      </c>
+      <c r="C3">
+        <v>44376</v>
+      </c>
+      <c r="D3" s="3">
+        <f>ROUND(Table1[[#This Row],[VSIZE]]/MIN(Table1[VSIZE]),1)</f>
+        <v>7</v>
+      </c>
+      <c r="E3" s="3">
+        <f>ROUND(Table1[[#This Row],[RSS]]/MIN(Table1[RSS]),1)</f>
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>3176236</v>
+      </c>
+      <c r="C4">
+        <v>36016</v>
+      </c>
+      <c r="D4" s="3">
+        <f>ROUND(Table1[[#This Row],[VSIZE]]/MIN(Table1[VSIZE]),1)</f>
+        <v>1</v>
+      </c>
+      <c r="E4" s="3">
+        <f>ROUND(Table1[[#This Row],[RSS]]/MIN(Table1[RSS]),1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5">
+        <v>22516000</v>
+      </c>
+      <c r="C5">
+        <v>59836</v>
+      </c>
+      <c r="D5" s="3">
+        <f>ROUND(Table1[[#This Row],[VSIZE]]/MIN(Table1[VSIZE]),1)</f>
+        <v>7.1</v>
+      </c>
+      <c r="E5" s="3">
+        <f>ROUND(Table1[[#This Row],[RSS]]/MIN(Table1[RSS]),1)</f>
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6">
+        <v>3401464</v>
+      </c>
+      <c r="C6">
+        <v>44148</v>
+      </c>
+      <c r="D6" s="3">
+        <f>ROUND(Table1[[#This Row],[VSIZE]]/MIN(Table1[VSIZE]),1)</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E6" s="3">
+        <f>ROUND(Table1[[#This Row],[RSS]]/MIN(Table1[RSS]),1)</f>
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" t="s">
+        <v>32</v>
+      </c>
+      <c r="H11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>337907.91</v>
+      </c>
+      <c r="C12">
+        <v>7.13</v>
+      </c>
+      <c r="D12">
+        <v>23413148</v>
+      </c>
+      <c r="E12">
+        <v>179924</v>
+      </c>
+      <c r="F12" s="3">
+        <f>ROUND(Table4[[#This Row],[VSIZE]]/MIN(Table4[VSIZE]),1)</f>
+        <v>5.3</v>
+      </c>
+      <c r="G12" s="3">
+        <f>ROUND(Table4[[#This Row],[RSS]]/MIN(Table4[RSS]),1)</f>
+        <v>3.3</v>
+      </c>
+      <c r="H12" s="3">
+        <f>ROUND(Table4[[#This Row],[RPS]]/MAX(Table4[RPS]),1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>289927.09000000003</v>
+      </c>
+      <c r="C13">
+        <v>8.11</v>
+      </c>
+      <c r="D13">
+        <v>4429680</v>
+      </c>
+      <c r="E13">
+        <v>54616</v>
+      </c>
+      <c r="F13" s="3">
+        <f>ROUND(Table4[[#This Row],[VSIZE]]/MIN(Table4[VSIZE]),1)</f>
+        <v>1</v>
+      </c>
+      <c r="G13" s="3">
+        <f>ROUND(Table4[[#This Row],[RSS]]/MIN(Table4[RSS]),1)</f>
+        <v>1</v>
+      </c>
+      <c r="H13" s="3">
+        <f>ROUND(Table4[[#This Row],[RPS]]/MAX(Table4[RPS]),1)</f>
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>28604.05</v>
+      </c>
+      <c r="C14">
+        <v>78.760000000000005</v>
+      </c>
+      <c r="D14">
+        <v>24388948</v>
+      </c>
+      <c r="E14">
+        <v>241156</v>
+      </c>
+      <c r="F14" s="3">
+        <f>ROUND(Table4[[#This Row],[VSIZE]]/MIN(Table4[VSIZE]),1)</f>
+        <v>5.5</v>
+      </c>
+      <c r="G14" s="3">
+        <f>ROUND(Table4[[#This Row],[RSS]]/MIN(Table4[RSS]),1)</f>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="H14" s="3">
+        <f>ROUND(Table4[[#This Row],[RPS]]/MAX(Table4[RPS]),1)</f>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>25405.41</v>
+      </c>
+      <c r="C15">
+        <v>90.32</v>
+      </c>
+      <c r="D15">
+        <v>5126948</v>
+      </c>
+      <c r="E15">
+        <v>112892</v>
+      </c>
+      <c r="F15" s="3">
+        <f>ROUND(Table4[[#This Row],[VSIZE]]/MIN(Table4[VSIZE]),1)</f>
+        <v>1.2</v>
+      </c>
+      <c r="G15" s="3">
+        <f>ROUND(Table4[[#This Row],[RSS]]/MIN(Table4[RSS]),1)</f>
+        <v>2.1</v>
+      </c>
+      <c r="H15" s="3">
+        <f>ROUND(Table4[[#This Row],[RPS]]/MAX(Table4[RPS]),1)</f>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="D3:D6">
+    <cfRule type="dataBar" priority="5">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF008AEF"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{487D37BA-7C6A-44C6-878C-229D48882387}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G12:G15">
+    <cfRule type="dataBar" priority="4">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF008AEF"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{F5592B91-1B9E-4360-95D5-FF6B786B0A49}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H12:H15">
+    <cfRule type="dataBar" priority="3">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF008AEF"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{C7DD537D-60B2-4F5D-8ECB-5B70F5833CCD}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3:E6">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF008AEF"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{5B2C8D25-9BAE-43A7-8B20-646023CED4C9}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F12:F15">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF008AEF"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{927B12BB-D9DF-41A5-9A6F-FD7CCFFE5222}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{487D37BA-7C6A-44C6-878C-229D48882387}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF008AEF"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D3:D6</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{F5592B91-1B9E-4360-95D5-FF6B786B0A49}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF008AEF"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>G12:G15</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{C7DD537D-60B2-4F5D-8ECB-5B70F5833CCD}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF008AEF"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>H12:H15</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{5B2C8D25-9BAE-43A7-8B20-646023CED4C9}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF008AEF"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E3:E6</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{927B12BB-D9DF-41A5-9A6F-FD7CCFFE5222}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF008AEF"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>F12:F15</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update to 2016/04/06 Linux CPU utilization
</commit_message>
<xml_diff>
--- a/results/2016-04-06/Summary.xlsx
+++ b/results/2016-04-06/Summary.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="36">
   <si>
     <t>Platform</t>
   </si>
@@ -129,8 +129,10 @@
     <t>ps -o rss,vsize,command -u asplab</t>
   </si>
   <si>
-    <t xml:space="preserve">wrk -c 256 -t 32 -d 10 -s ./scripts/pipeline.lua http://10.194.217.77:5000/ -- 16
-</t>
+    <t>top</t>
+  </si>
+  <si>
+    <t>wrk -c 256 -t 32 -d 10 -s ./scripts/pipeline.lua http://10.194.217.77:5000/ -- 16</t>
   </si>
 </sst>
 </file>
@@ -2701,7 +2703,7 @@
     <tableColumn id="5" name="Ratio vs Best (VSIZE)" dataDxfId="4">
       <calculatedColumnFormula>ROUND(Table1[[#This Row],[VSIZE]]/MIN(Table1[VSIZE]),1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Ratio vs Best (RSS)" dataDxfId="1">
+    <tableColumn id="6" name="Ratio vs Best (RSS)" dataDxfId="3">
       <calculatedColumnFormula>ROUND(Table1[[#This Row],[RSS]]/MIN(Table1[RSS]),1)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2718,15 +2720,27 @@
     <tableColumn id="3" name="Avg latency (ms)"/>
     <tableColumn id="4" name="VSIZE"/>
     <tableColumn id="5" name="RSS"/>
-    <tableColumn id="7" name="Ratio vs Best (VSIZE)" dataDxfId="0">
+    <tableColumn id="7" name="Ratio vs Best (VSIZE)" dataDxfId="2">
       <calculatedColumnFormula>ROUND(Table4[[#This Row],[VSIZE]]/MIN(Table4[VSIZE]),1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Ratio vs Best (RSS)" dataDxfId="3">
+    <tableColumn id="8" name="Ratio vs Best (RSS)" dataDxfId="1">
       <calculatedColumnFormula>ROUND(Table4[[#This Row],[RSS]]/MIN(Table4[RSS]),1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Ratio vs Best (RPS)" dataDxfId="2">
+    <tableColumn id="9" name="Ratio vs Best (RPS)" dataDxfId="0">
       <calculatedColumnFormula>ROUND(Table4[[#This Row],[RPS]]/MAX(Table4[RPS]),1)</calculatedColumnFormula>
     </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A20:C24" totalsRowShown="0">
+  <autoFilter ref="A20:C24"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Platform"/>
+    <tableColumn id="2" name="Command"/>
+    <tableColumn id="3" name="Server CPU utilization"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3031,15 +3045,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
-    </sheetView>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.140625" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.85546875" customWidth="1"/>
     <col min="5" max="5" width="19.5703125" customWidth="1"/>
     <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
@@ -3660,7 +3672,7 @@
       <c r="A30" s="5"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -3913,15 +3925,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="46.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.85546875" customWidth="1"/>
     <col min="2" max="2" width="13.140625" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
     <col min="6" max="6" width="21.42578125" bestFit="1" customWidth="1"/>
@@ -4175,20 +4187,83 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="7">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="7">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="7">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" s="7">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>33</v>
       </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="2"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3:D6">
@@ -4263,9 +4338,10 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <tableParts count="2">
+  <tableParts count="3">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">

</xml_diff>